<commit_message>
nuke demo nkde design
</commit_message>
<xml_diff>
--- a/NKDEDesign.xlsx
+++ b/NKDEDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I566225/SAPDevelop/projects/nuke-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80142F56-E69D-844D-9B74-61739896FAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53562980-3074-1649-BB45-022A9DACC26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="520" windowWidth="76800" windowHeight="29800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NKDEDesign" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="60">
   <si>
     <t>symbol</t>
   </si>
@@ -188,6 +188,36 @@
   </si>
   <si>
     <t>StepComplition listener writes agregated  metadata for 3ss files.</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>architecture</t>
+  </si>
+  <si>
+    <t>purpose and use cases</t>
+  </si>
+  <si>
+    <t>Classic project setup and resources sharing (services are shared between batch spring boot) gradle.</t>
+  </si>
+  <si>
+    <t>Batch bonuses spring integration and extension.</t>
+  </si>
+  <si>
+    <t>Data flow (Partitioner &gt; Reader &gt; Processor &gt; Writer) and commit interval</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Solution implementation</t>
+  </si>
+  <si>
+    <t>MCS benefits.</t>
   </si>
 </sst>
 </file>
@@ -17267,646 +17297,18 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="3365500" y="7924800"/>
-          <a:ext cx="2514600" cy="2336800"/>
-          <a:chOff x="4292600" y="18211800"/>
-          <a:chExt cx="2476500" cy="2336800"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4889500" y="18211800"/>
-            <a:ext cx="1879600" cy="2336800"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="2800">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>REDIS</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>SESSION STORE</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 3" descr="Redis icon">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm flipH="1">
-            <a:off x="4292600" y="18681700"/>
-            <a:ext cx="1422400" cy="1422400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>616848</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="Group 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="7556500" y="7518400"/>
-          <a:ext cx="2293248" cy="3632200"/>
-          <a:chOff x="7028553" y="2298700"/>
-          <a:chExt cx="2267848" cy="3632200"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7416801" y="2298700"/>
-            <a:ext cx="1879600" cy="3632200"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="2800">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>KAFKA</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> CLUSTER</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1600" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>MESSAGE BROKER</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="7" name="Picture 6" descr="Running Apache Kafka on Windows 10 | by Bivás Biswas | Towards ...">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm rot="5400000">
-            <a:off x="6524932" y="3310330"/>
-            <a:ext cx="2621794" cy="1614551"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:duotone>
-            <a:schemeClr val="bg2">
-              <a:shade val="45000"/>
-              <a:satMod val="135000"/>
-            </a:schemeClr>
-            <a:prstClr val="white"/>
-          </a:duotone>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4826000" y="2451100"/>
-          <a:ext cx="3251200" cy="3251200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>585470</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Graphic 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId5"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11709400" y="3479800"/>
-          <a:ext cx="4560570" cy="1689100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:effectLst>
-          <a:glow rad="228600">
-            <a:schemeClr val="bg1">
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:glow>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>154859</xdr:rowOff>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>65959</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17922,10 +17324,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId7"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -17935,8 +17337,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5334000" y="6350000"/>
-          <a:ext cx="2628900" cy="713659"/>
+          <a:off x="2743200" y="2603500"/>
+          <a:ext cx="2667000" cy="713659"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18850,7 +18252,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
@@ -18873,8 +18275,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15913100" y="20764500"/>
-          <a:ext cx="14071600" cy="15798800"/>
+          <a:off x="15621000" y="20764500"/>
+          <a:ext cx="14363700" cy="15798800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -21134,16 +20536,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>231</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21158,7 +20560,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9232900" y="44297600"/>
+          <a:off x="10769600" y="39700200"/>
           <a:ext cx="2679700" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -21247,28 +20649,26 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-GB" sz="1800">
+            <a:rPr lang="en-US" sz="1800" b="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Registers</a:t>
+            <a:t>If</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1800" baseline="0">
+            <a:rPr lang="en-US" sz="1800" b="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> all available jobs. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Responsible for persisting the state of job executions and step executions.</a:t>
+            <a:t> all properly set you can view, conficgure and launch batch through Batch Admin that provides UI out of the box.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400" b="0">
             <a:solidFill>
@@ -21315,8 +20715,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21332,7 +20732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12496800" y="22021800"/>
-          <a:ext cx="2679700" cy="3124200"/>
+          <a:ext cx="2679700" cy="4610100"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -21427,6 +20827,1552 @@
             </a:rPr>
             <a:t>A Job represents the entire batch process. It consists of multiple steps and defines the sequence in which those steps should be executed.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1800" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Job Execution State is persisted.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="115" name="Rounded Rectangle 114">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78879483-5F7A-7D4D-AE40-65629DC72746}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12547600" y="27012900"/>
+          <a:ext cx="2679700" cy="1879600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>JobScope</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Initiates the execution of a job</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and passes necessary parmeters.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="116" name="Rounded Rectangle 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDED18A6-639D-B54B-87DC-5B37C3261201}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12560300" y="29286200"/>
+          <a:ext cx="2679700" cy="1879600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>JobListener</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Initiates the execution of a job</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and passes necessary parmeters.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="117" name="Rounded Rectangle 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A2F8D1-5680-F246-B42D-1D78438AA67E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16040100" y="22110700"/>
+          <a:ext cx="2679700" cy="4610100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Flow</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>A Flow is a sequence of steps or transitions within a job. It can be used to model complex job flows, including conditional transitions, splits, and joins.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="118" name="Rounded Rectangle 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5345DFC-479A-1A47-A008-67D84475739B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16040100" y="27063700"/>
+          <a:ext cx="2679700" cy="3365500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FlowBuilder</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Split, Join and decide on a condition.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>A decision controller that determines the next step to execute based on the result of the previous step. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="Rounded Rectangle 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6753C219-CC94-054B-96B5-9640F73E9F43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19177000" y="22085300"/>
+          <a:ext cx="2679700" cy="2730500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Step</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>A Step is a single phase of a job. It defines the actual work to be done, including partitioning, reading, processing, and writing data.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="120" name="Rounded Rectangle 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFA47C4-CED8-644D-996A-79A3AB605464}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19202400" y="26022300"/>
+          <a:ext cx="2679700" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>StepListener</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="Rounded Rectangle 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D69E4099-4F8F-FC44-A305-44340CCF3A53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19202400" y="25095200"/>
+          <a:ext cx="2679700" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>StepScope</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="122" name="Rounded Rectangle 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C61ED47C-4A0E-4542-8807-CEDA7EF33201}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24726900" y="21526500"/>
+          <a:ext cx="4127500" cy="1739900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Partitioner</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Divides data into smaller chunks for parallel processing. It improves the performance by processing partitions concurrently.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="123" name="Rounded Rectangle 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E89ADCB-4020-214A-AA75-567B3070C10A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14262100" y="37795200"/>
+          <a:ext cx="2679700" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Transaction manager</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="124" name="Rounded Rectangle 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E42E3A-1C69-3348-AE90-A27B3984BE0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17538700" y="37769800"/>
+          <a:ext cx="2679700" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Observability</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="Rounded Rectangle 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28A2418E-3359-894C-AAEB-833CFEACB961}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20764500" y="37795200"/>
+          <a:ext cx="2679700" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent6">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="37000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Interceptors</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Before job, before step Spring</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> common toolset</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
               <a:solidFill>
@@ -23919,10 +24865,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="D8:Y88"/>
+  <dimension ref="U14:Y88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C89" workbookViewId="0">
-      <selection activeCell="N91" sqref="N91"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AD191" sqref="AD191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23931,15 +24877,84 @@
     <col min="22" max="22" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D8">
-        <v>1000000000</v>
+    <row r="14" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D9">
-        <f>D8/300</f>
-        <v>3333333.3333333335</v>
+    <row r="15" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <v>3</v>
+      </c>
+      <c r="V16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U17">
+        <v>4</v>
+      </c>
+      <c r="V17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U18">
+        <v>5</v>
+      </c>
+      <c r="V18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U19">
+        <v>6</v>
+      </c>
+      <c r="V19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U20">
+        <v>7</v>
+      </c>
+      <c r="V20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U21">
+        <v>8</v>
+      </c>
+      <c r="V21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U22">
+        <v>9</v>
+      </c>
+      <c r="V22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U23">
+        <v>10</v>
+      </c>
+      <c r="V23" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="21:25" x14ac:dyDescent="0.2">

</xml_diff>